<commit_message>
Two more source summaries
</commit_message>
<xml_diff>
--- a/Study table.xlsx
+++ b/Study table.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="28">
   <si>
     <t>Study</t>
   </si>
   <si>
-    <t>Analytical only</t>
-  </si>
-  <si>
     <t>Steady State</t>
   </si>
   <si>
@@ -80,9 +77,6 @@
     <t>Heating</t>
   </si>
   <si>
-    <t>Absorbtion cooling</t>
-  </si>
-  <si>
     <t>Cascading to lower temp processes</t>
   </si>
   <si>
@@ -102,13 +96,25 @@
   </si>
   <si>
     <t>Regenerative ORC</t>
+  </si>
+  <si>
+    <t>A review of Organic Rankine cycles (ORCs) for the recovery of low-grade waste heat</t>
+  </si>
+  <si>
+    <t>Analytical</t>
+  </si>
+  <si>
+    <t>Application of waste heat powered absorption refrigeration system to the LNG recovery process</t>
+  </si>
+  <si>
+    <t>Absorption cooling</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +127,12 @@
       <color rgb="FF00B050"/>
       <name val="Wingdings"/>
       <charset val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -201,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -221,6 +233,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,7 +540,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -537,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,12 +576,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="8"/>
       <c r="E1" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
@@ -576,88 +589,88 @@
       <c r="I1" s="7"/>
       <c r="J1" s="8"/>
       <c r="K1" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
       <c r="N1" s="8"/>
       <c r="O1" s="4"/>
       <c r="P1" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q1" s="5"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="K2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="O2" s="2"/>
       <c r="P2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="1"/>
       <c r="D3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -669,34 +682,34 @@
     </row>
     <row r="4" spans="1:17" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -704,13 +717,13 @@
     </row>
     <row r="5" spans="1:17" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -719,7 +732,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -727,22 +740,22 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -754,34 +767,34 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q6" s="1"/>
     </row>
     <row r="7" spans="1:17" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -791,36 +804,45 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1"/>
+    <row r="8" spans="1:17" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
+      <c r="P8" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1"/>
+    <row r="9" spans="1:17" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -831,10 +853,14 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
+      <c r="M9" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
+      <c r="P9" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
First draft of proposal with integrated preliminary results
</commit_message>
<xml_diff>
--- a/Study table.xlsx
+++ b/Study table.xlsx
@@ -24,18 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="26">
   <si>
     <t>Study</t>
-  </si>
-  <si>
-    <t>Steady State</t>
-  </si>
-  <si>
-    <t>Transient</t>
-  </si>
-  <si>
-    <t>Time</t>
   </si>
   <si>
     <t>Type</t>
@@ -223,8 +214,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -236,6 +225,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -543,7 +538,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -551,182 +546,165 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="7" t="s">
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="7"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q1" s="6"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="2" t="s">
+      <c r="M2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="1"/>
       <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:17" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
+    </row>
+    <row r="4" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:17" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -735,30 +713,25 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q5" s="1"/>
-    </row>
-    <row r="6" spans="1:17" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>20</v>
+    </row>
+    <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -768,36 +741,31 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="1:17" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>21</v>
+    </row>
+    <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -805,26 +773,21 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q7" s="1"/>
-    </row>
-    <row r="8" spans="1:17" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>24</v>
+    </row>
+    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -833,18 +796,13 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q8" s="1"/>
-    </row>
-    <row r="9" spans="1:17" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>26</v>
+    </row>
+    <row r="9" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -857,55 +815,45 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q9" s="1"/>
-    </row>
-    <row r="10" spans="1:17" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>28</v>
+    </row>
+    <row r="10" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="O10" s="1"/>
-      <c r="P10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q10" s="1"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -922,11 +870,8 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -943,11 +888,8 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -964,11 +906,8 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -985,11 +924,8 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1006,11 +942,8 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1027,11 +960,8 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1048,13 +978,9 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="P1:Q1"/>
+  <mergeCells count="4">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:J1"/>

</xml_diff>

<commit_message>
Several source summaries and proposal progress
</commit_message>
<xml_diff>
--- a/Study table.xlsx
+++ b/Study table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="29">
   <si>
     <t>Study</t>
   </si>
@@ -102,6 +102,15 @@
   </si>
   <si>
     <t>BCS I Waste heat recovery technology and opportunities in US industry</t>
+  </si>
+  <si>
+    <t>New Turbo Compound Systems in Automotive Industry for Internal Combustion Engine to Recover Energy</t>
+  </si>
+  <si>
+    <t>Kinetic energy recovery (Turbo)</t>
+  </si>
+  <si>
+    <t>Comparison of Thermodynamic Cycles for Power Production from Low-temperature Geothermal Heat Sources</t>
   </si>
 </sst>
 </file>
@@ -214,6 +223,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -225,12 +240,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -546,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:N10"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,35 +576,37 @@
     <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="34.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="5" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="5" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="7"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="9"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -633,11 +644,14 @@
         <v>24</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3"/>
@@ -663,9 +677,10 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1"/>
@@ -692,12 +707,13 @@
       <c r="M4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="N4" s="3"/>
+      <c r="O4" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -719,9 +735,10 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -741,9 +758,10 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -773,9 +791,10 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -795,10 +814,10 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-      <c r="N8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -817,10 +836,11 @@
       <c r="M9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="N9" s="3"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="1"/>
@@ -849,16 +869,19 @@
       <c r="M10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N10" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>9</v>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="C11" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -869,27 +892,47 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="N11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+      <c r="F12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -906,8 +949,9 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -924,8 +968,9 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -942,8 +987,9 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -960,8 +1006,9 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -978,13 +1025,204 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:J1"/>
-    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="K1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Draft of proposal power point
</commit_message>
<xml_diff>
--- a/Study table.xlsx
+++ b/Study table.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clappg\Documents\GitHub\Masters_Thesis\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64668F1-DAD4-4CF5-A286-68527E791D45}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -105,9 +99,6 @@
     <t>Application of waste heat powered absorption refrigeration system to the LNG recovery process</t>
   </si>
   <si>
-    <t>Absorption cooling</t>
-  </si>
-  <si>
     <t>BCS I Waste heat recovery technology and opportunities in US industry</t>
   </si>
   <si>
@@ -142,12 +133,15 @@
   </si>
   <si>
     <t>Multi-criteria evaluation of several million working fluids for waste heat recovery by means of organic rankine cycle in passenger cars and heavy duty trucks</t>
+  </si>
+  <si>
+    <t>Absorpsion cooling</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -578,18 +572,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,10 +666,10 @@
         <v>13</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>14</v>
@@ -874,7 +868,7 @@
     </row>
     <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -909,7 +903,7 @@
     </row>
     <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
@@ -932,7 +926,7 @@
     </row>
     <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>4</v>
@@ -967,7 +961,7 @@
     </row>
     <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>4</v>
@@ -992,7 +986,7 @@
     </row>
     <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1019,7 +1013,7 @@
     </row>
     <row r="15" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>4</v>
@@ -1048,7 +1042,7 @@
     </row>
     <row r="16" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>4</v>
@@ -1075,7 +1069,7 @@
     </row>
     <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
@@ -1104,7 +1098,7 @@
     </row>
     <row r="18" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1135,7 +1129,7 @@
     </row>
     <row r="19" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>4</v>
@@ -1168,7 +1162,7 @@
     </row>
     <row r="20" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>4</v>

</xml_diff>